<commit_message>
fix calc and table
</commit_message>
<xml_diff>
--- a/lvl.xlsx
+++ b/lvl.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurii/Desktop/Work/ZP_GOZ/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBD9D03-9AEE-7143-A095-C4E09B76A24B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="18195" windowHeight="11310"/>
+    <workbookView xWindow="1480" yWindow="4860" windowWidth="18200" windowHeight="11320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>дневные</t>
   </si>
@@ -29,11 +35,17 @@
   <si>
     <t>отхожено ночных</t>
   </si>
+  <si>
+    <t>часы</t>
+  </si>
+  <si>
+    <t>проценты</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -75,6 +87,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -123,7 +138,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -156,9 +171,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -191,6 +223,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -366,20 +415,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D6:L10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="D5:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="2.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="2.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>0</v>
       </c>
@@ -407,7 +464,7 @@
         <v>905.44999999999993</v>
       </c>
     </row>
-    <row r="7" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
         <v>1</v>
       </c>
@@ -439,7 +496,7 @@
         <v>1999.94</v>
       </c>
     </row>
-    <row r="8" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
         <v>2</v>
       </c>
@@ -447,7 +504,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
         <v>3</v>
       </c>
@@ -459,7 +516,7 @@
         <v>180.89999999999998</v>
       </c>
     </row>
-    <row r="10" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:12" x14ac:dyDescent="0.2">
       <c r="F10">
         <v>2000</v>
       </c>
@@ -470,24 +527,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add favicon and upgrade lvl calc
</commit_message>
<xml_diff>
--- a/lvl.xlsx
+++ b/lvl.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurii/Desktop/Work/ZP_GOZ/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\ZP_GOZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBD9D03-9AEE-7143-A095-C4E09B76A24B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DB6B6E-03F9-4357-8A93-899E88B4EF06}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="4860" windowWidth="18200" windowHeight="11320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1485" yWindow="4860" windowWidth="18195" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -416,19 +416,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D5:L10"/>
+  <dimension ref="D5:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="2.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>4</v>
       </c>
@@ -436,7 +436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>0</v>
       </c>
@@ -464,7 +464,7 @@
         <v>905.44999999999993</v>
       </c>
     </row>
-    <row r="7" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>1</v>
       </c>
@@ -496,7 +496,7 @@
         <v>1999.94</v>
       </c>
     </row>
-    <row r="8" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>2</v>
       </c>
@@ -504,7 +504,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>3</v>
       </c>
@@ -516,9 +516,29 @@
         <v>180.89999999999998</v>
       </c>
     </row>
-    <row r="10" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F10">
         <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <f>ROUND(H6/F6, 2)</f>
+        <v>11.06</v>
+      </c>
+      <c r="J12">
+        <f>I12*F6</f>
+        <v>905.81399999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <f>ROUND(H7/F7, 2)</f>
+        <v>11.06</v>
+      </c>
+      <c r="J13">
+        <f>I13*F7</f>
+        <v>1094.94</v>
       </c>
     </row>
   </sheetData>
@@ -532,7 +552,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -544,7 +564,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add normal lvl calc in table
</commit_message>
<xml_diff>
--- a/lvl.xlsx
+++ b/lvl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\ZP_GOZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DB6B6E-03F9-4357-8A93-899E88B4EF06}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246EC1FA-DA93-4D57-83BF-FA6EAD1E044A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1485" yWindow="4860" windowWidth="18195" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,13 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>дневные</t>
-  </si>
-  <si>
-    <t>ночные</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>отхожено дневных</t>
   </si>
@@ -40,6 +34,15 @@
   </si>
   <si>
     <t>проценты</t>
+  </si>
+  <si>
+    <t>дневные по графику</t>
+  </si>
+  <si>
+    <t>ночные по графику</t>
+  </si>
+  <si>
+    <t>дни</t>
   </si>
 </sst>
 </file>
@@ -418,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D5:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,44 +432,47 @@
   </cols>
   <sheetData>
     <row r="5" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
       <c r="F5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6">
         <f>E6*11.7</f>
-        <v>81.899999999999991</v>
+        <v>70.199999999999989</v>
       </c>
       <c r="G6">
         <f>F6/(F9/100)</f>
-        <v>45.273631840796021</v>
+        <v>41.489361702127653</v>
       </c>
       <c r="H6">
         <f>G6/100*F10</f>
-        <v>905.4726368159204</v>
+        <v>829.78723404255311</v>
       </c>
       <c r="I6">
         <f>ROUND(H6/E6, 2)</f>
-        <v>129.35</v>
+        <v>138.30000000000001</v>
       </c>
       <c r="J6">
         <f>I6*E8</f>
-        <v>905.44999999999993</v>
+        <v>829.80000000000007</v>
       </c>
     </row>
     <row r="7" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E7">
         <v>9</v>
@@ -477,43 +483,43 @@
       </c>
       <c r="G7">
         <f>F7/(F9/100)</f>
-        <v>54.726368159203986</v>
+        <v>58.51063829787234</v>
       </c>
       <c r="H7">
         <f>G7/100*F10</f>
-        <v>1094.5273631840798</v>
+        <v>1170.2127659574469</v>
       </c>
       <c r="I7">
         <f>ROUND(H7/E7, 2)</f>
-        <v>121.61</v>
+        <v>130.02000000000001</v>
       </c>
       <c r="J7">
         <f>I7*E9</f>
-        <v>1094.49</v>
+        <v>780.12000000000012</v>
       </c>
       <c r="L7">
         <f>J6+J7</f>
-        <v>1999.94</v>
+        <v>1609.92</v>
       </c>
     </row>
     <row r="8" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F9">
         <f>F6+F7</f>
-        <v>180.89999999999998</v>
+        <v>169.2</v>
       </c>
     </row>
     <row r="10" spans="4:12" x14ac:dyDescent="0.25">
@@ -522,23 +528,35 @@
       </c>
     </row>
     <row r="12" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f>E8*11.7</f>
+        <v>70.199999999999989</v>
+      </c>
       <c r="I12">
         <f>ROUND(H6/F6, 2)</f>
-        <v>11.06</v>
+        <v>11.82</v>
       </c>
       <c r="J12">
-        <f>I12*F6</f>
-        <v>905.81399999999996</v>
+        <f>I12*F12</f>
+        <v>829.7639999999999</v>
       </c>
     </row>
     <row r="13" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f>E9*11</f>
+        <v>66</v>
+      </c>
       <c r="I13">
         <f>ROUND(H7/F7, 2)</f>
-        <v>11.06</v>
+        <v>11.82</v>
       </c>
       <c r="J13">
-        <f>I13*F7</f>
-        <v>1094.94</v>
+        <f>I13*F13</f>
+        <v>780.12</v>
+      </c>
+      <c r="L13">
+        <f>J12+J13</f>
+        <v>1609.884</v>
       </c>
     </row>
   </sheetData>

</xml_diff>